<commit_message>
Finally :'( I did it.... over 300 changes
1000 LINES OF CODE YEAH
</commit_message>
<xml_diff>
--- a/2 - Scaling plus Rotation/Scrotation Analysis Template.xlsx
+++ b/2 - Scaling plus Rotation/Scrotation Analysis Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emban\Documents\GitHub\EMC-Scrotation-Station\2 - Scaling plus Rotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4FF502-0C6F-41A5-AA96-A4521855CB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7FF195-3D0E-4BA4-88F0-EB5C38DA4BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Colors</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Angle of Roll (°)</t>
+  </si>
+  <si>
+    <t>Absolute Angle of Roll (|°|)</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -522,13 +525,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
         <v>6</v>
@@ -545,7 +548,7 @@
         <v>19</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -555,15 +558,17 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J4" t="s">
         <v>6</v>

</xml_diff>